<commit_message>
end2end_refund qr code payment
</commit_message>
<xml_diff>
--- a/FolderExcelFiles/I - SUBCRIBER/3. Transactions/transfer/transfer to wallet/1. Transfer - To - Wallet- Success.xlsx
+++ b/FolderExcelFiles/I - SUBCRIBER/3. Transactions/transfer/transfer to wallet/1. Transfer - To - Wallet- Success.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Downloads\AYA Subscriber App\FolderExcelFiles\I - SUBCRIBER\3. Transactions\transfer\transfer to wallet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7C5C3D-01F1-4703-93D9-1852DC523D23}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE74DDC-916D-4F9E-AA0E-4DB15CE37DF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1432A72A-0386-441C-9E35-C35EB92B75C6}"/>
   </bookViews>
@@ -84,9 +84,6 @@
     <t>customer</t>
   </si>
   <si>
-    <t>09686021096</t>
-  </si>
-  <si>
     <t>MMK</t>
   </si>
   <si>
@@ -103,6 +100,9 @@
   </si>
   <si>
     <t>OTP</t>
+  </si>
+  <si>
+    <t>09506569643</t>
   </si>
 </sst>
 </file>
@@ -480,7 +480,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,8 +488,8 @@
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
     <col min="8" max="8" width="18.5703125" customWidth="1"/>
@@ -506,7 +506,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -545,7 +545,7 @@
         <v>15</v>
       </c>
       <c r="O1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P1" t="s">
         <v>3</v>
@@ -556,7 +556,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
@@ -575,22 +575,22 @@
         <v>18</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="J2" s="3">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="N2" t="str">
         <f>B2</f>

</xml_diff>